<commit_message>
Added display of missing block types.
</commit_message>
<xml_diff>
--- a/Bildmaterial/Block map.xlsx
+++ b/Bildmaterial/Block map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
   <si>
     <t>S</t>
   </si>
@@ -27,9 +27,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>HORIZONTAL</t>
   </si>
   <si>
-    <t>EDGE</t>
-  </si>
-  <si>
     <t>VERTICAL</t>
   </si>
   <si>
@@ -109,6 +103,30 @@
   </si>
   <si>
     <t>GOAL BLACK</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>EDGE UP</t>
+  </si>
+  <si>
+    <t>EDGE RIGHT</t>
+  </si>
+  <si>
+    <t>EDGE DOWN</t>
+  </si>
+  <si>
+    <t>EDGE LEFT</t>
   </si>
 </sst>
 </file>
@@ -325,21 +343,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -347,13 +386,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -439,6 +471,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
@@ -446,6 +499,92 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
@@ -453,6 +592,92 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -467,14 +692,86 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -754,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:W17"/>
+  <dimension ref="D2:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -770,644 +1067,817 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
       <c r="O3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="O4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
       <c r="O5" s="5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+        <v>29</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="O6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="O7" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="O8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
       <c r="O9" s="5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="O10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W10" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
       <c r="O11" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
       <c r="O12" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W12" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
       <c r="O13" s="5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
       <c r="O14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
       <c r="O15" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="W15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="W15" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
       <c r="O16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S16" s="6" t="s">
         <v>1</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="4:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
       <c r="O17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="T17" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U17" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V17" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W17" s="10" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F6:J6"/>
+  <mergeCells count="18">
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F9:J9"/>
     <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F18:J18"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="F16:J16"/>
     <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F4:J4"/>
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F4:J4"/>
     <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F7:J7"/>
   </mergeCells>
+  <conditionalFormatting sqref="A28:XFD1048576 A21:AF27 K16:AF20 AN16:XFD27 D9:J20 A1:XFD4 A5:C20 K5:XFD15 D6:J6">
+    <cfRule type="cellIs" dxfId="54" priority="43" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="44" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="45" operator="equal">
+      <formula>"GB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="46" operator="equal">
+      <formula>"GY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="47" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="48" operator="equal">
+      <formula>"GR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>"BB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+      <formula>"BY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="51" operator="equal">
+      <formula>"BG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="52" operator="equal">
+      <formula>"BR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
+      <formula>"E"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="55" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:J5">
+    <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="31" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="32" operator="equal">
+      <formula>"GB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="33" operator="equal">
+      <formula>"GY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
+      <formula>"GR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+      <formula>"BB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
+      <formula>"BY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
+      <formula>"BG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
+      <formula>"BR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
+      <formula>"E"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="42" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:J7">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+      <formula>"GB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+      <formula>"GY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"GR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"BB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"BY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+      <formula>"BG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+      <formula>"BR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
+      <formula>"E"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="29" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:J8">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>"W"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"GB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"GY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"GR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"BB"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"BY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+      <formula>"BG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+      <formula>"BR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
-      <formula>"S"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
-      <formula>"E"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
-      <formula>"BR"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"BG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"BY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"BB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"GR"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"GG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>"GY"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
-      <formula>"GB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
-      <formula>"W"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"N"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"ER"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"ED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"EL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"EU"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First attempts at moving figures (incomlete)
</commit_message>
<xml_diff>
--- a/Bildmaterial/Block map.xlsx
+++ b/Bildmaterial/Block map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="38">
   <si>
     <t>S</t>
   </si>
@@ -27,9 +27,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>START</t>
   </si>
   <si>
-    <t>HORIZONTAL</t>
-  </si>
-  <si>
     <t>VERTICAL</t>
   </si>
   <si>
@@ -127,6 +121,18 @@
   </si>
   <si>
     <t>EDGE LEFT</t>
+  </si>
+  <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HORIZONTAL LEFT</t>
+  </si>
+  <si>
+    <t>HORIZONTAL RIGHT</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:W20"/>
+  <dimension ref="D2:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1062,650 +1068,701 @@
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="O3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="T3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>12</v>
+      <c r="Y3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
-      <c r="O4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" s="6" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="T4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>13</v>
+      <c r="Y4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="O5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>2</v>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="T5" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="O6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>5</v>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="T6" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="7" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="O7" s="5" t="s">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="T7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="8" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="O8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>5</v>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="T8" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
-      <c r="O9" s="5" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="T9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="6" t="s">
+    </row>
+    <row r="10" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F10" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
-      <c r="O10" s="5" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="T10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W10" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F11" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
-      <c r="O11" s="5" t="s">
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="T11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W11" s="7" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="12" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
-      <c r="O12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>5</v>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="T12" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W12" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="O13" s="5" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="T13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="14" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
-      <c r="O14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>5</v>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="T14" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="15" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
-      <c r="O15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>2</v>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="T15" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="W15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB15" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
-      <c r="O16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q16" s="6" t="s">
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="T16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R16" s="6" t="s">
+      <c r="U16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="S16" s="6" t="s">
+      <c r="V16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="V16" s="6" t="s">
+      <c r="Y16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W16" s="7" t="s">
+      <c r="Z16" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="AA16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="4:23" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:28" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
-      <c r="O17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q17" s="9" t="s">
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="T17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="U17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="S17" s="9" t="s">
+      <c r="V17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="T17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="U17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="V17" s="9" t="s">
+      <c r="Y17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="W17" s="10" t="s">
+      <c r="Z17" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="AA17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB17" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="4:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="4:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F11:J11"/>
+  <mergeCells count="19">
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="F15:L15"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="F13:L13"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="F20:L20"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="F17:L17"/>
+    <mergeCell ref="F16:L16"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="F21:L21"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="F6:L6"/>
   </mergeCells>
-  <conditionalFormatting sqref="A28:XFD1048576 A21:AF27 K16:AF20 AN16:XFD27 D9:J20 A1:XFD4 A5:C20 K5:XFD15 D6:J6">
+  <conditionalFormatting sqref="A38:XFD1048576 A22:AF22 AN17:XFD28 A6:C21 D7:F7 O23:AF28 O29:XFD37 X18:AF18 A1:XFD2 AC3:XFD16 AC17:AF17 A23:E37 A3:F5 M19:AF21 D10:F21 M3:N18 T3:AB17">
     <cfRule type="cellIs" dxfId="54" priority="43" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1746,7 +1803,7 @@
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:J5">
+  <conditionalFormatting sqref="D6:F6">
     <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1787,7 +1844,7 @@
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:J7">
+  <conditionalFormatting sqref="D8:F8">
     <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1828,7 +1885,7 @@
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:J8">
+  <conditionalFormatting sqref="D9:F9">
     <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1866,15 +1923,15 @@
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"ER"</formula>
+  <conditionalFormatting sqref="A1:XFD2 X18:XFD18 A38:XFD1048576 A23:E37 O23:XFD37 A22:XFD22 M19:XFD21 A3:F21 M3:N18 T3:XFD17">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"EL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"ED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"EL"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"ER"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"EU"</formula>

</xml_diff>